<commit_message>
Improved structure of thesis, small additions
</commit_message>
<xml_diff>
--- a/thesis/images/Statistics.xlsx
+++ b/thesis/images/Statistics.xlsx
@@ -224,10 +224,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -342,15 +342,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
+      <xdr:colOff>523876</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>176211</xdr:rowOff>
+      <xdr:rowOff>176209</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -659,7 +659,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:K24"/>
+  <dimension ref="C2:K19"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -715,23 +715,23 @@
         <v>4.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="24" spans="3:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="9" t="s">
+    <row r="19" spans="3:11" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C2:K2"/>
-    <mergeCell ref="C24:K24"/>
+    <mergeCell ref="C19:K19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>